<commit_message>
Update build + revert test
</commit_message>
<xml_diff>
--- a/.translate/novel_01.xlsx
+++ b/.translate/novel_01.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="227">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -212,9 +212,6 @@
   </si>
   <si>
     <t xml:space="preserve">目次</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mokuji</t>
   </si>
   <si>
     <t xml:space="preserve">3</t>
@@ -2402,7 +2399,7 @@
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="100"/>
@@ -2493,840 +2490,837 @@
       <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="64" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="112" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="64" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="96" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="64" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="64" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="80" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="64" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="64" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B64" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B69" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B89" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B91" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B92" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B96" s="3" t="s">
         <v>191</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B98" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B101" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B104" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B106" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B107" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B108" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="32" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B110" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B113" s="3" t="s">
         <v>224</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>